<commit_message>
data sheet urls included in documents
</commit_message>
<xml_diff>
--- a/data/AI_products.xlsx
+++ b/data/AI_products.xlsx
@@ -10122,7 +10122,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/datasheet_mgc_r2.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10163,7 +10163,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/110-0029208a_datasheet_mgc_r3gc_jan23.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10204,7 +10204,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/110-0029200a_datasheet_mgc_r2gc_jan23.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10275,7 +10275,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/datasheet_mgc_r3.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10353,7 +10353,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/datasheet_mgc_r4.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10452,7 +10452,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/datasheet_mgc_r5.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10506,7 +10506,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/9c7466e11a8d427bb564104e1a0a9f4a/datasheet_mgc_r1gc.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10636,7 +10636,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144_oem.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10697,7 +10697,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr189mk2portable.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr179mk2fcc_aug22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144_personal.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10863,7 +10863,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr179mkii.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10904,7 +10904,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144fcc_sep22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -10945,7 +10945,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr179mk2fccportable_aug22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11006,7 +11006,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144_submersible.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11066,7 +11066,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr179mk2portable.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11139,7 +11139,7 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144fcc_submersible_sep22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11180,7 +11180,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr189mk2_fcc_aug22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11238,7 +11238,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144_uav_jun23.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11303,7 +11303,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr189mk2.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11352,7 +11352,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr144fcc_oem_aug22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11410,7 +11410,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/a1b8bf7c95d84236a8089a8a691a0e6d/datasheet_mbr189mk2fccportable_aug22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11473,7 +11473,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/5d74ac17037e48d383900f89d4f9557b/482731a-topas-ps120-datasheet.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11514,7 +11514,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/globalassets/maritime/km-products/product-documents/topas-ps-18-parametric-sub-bottom-profiler.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11579,7 +11579,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/globalassets/maritime/km-products/product-documents/topas-ps-40-parametric-sub-bottom-profiler.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11653,7 +11653,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/c22a596095db4994a5f26ba216b6b968/110-0017978a_datasheet_seapath380_dec22.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11718,7 +11718,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/c22a596095db4994a5f26ba216b6b968/110-0017979b_datasheet_seapath380-r_series.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11787,7 +11787,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/c22a596095db4994a5f26ba216b6b968/110-0034148a_datasheet_seapath130_apr23.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11843,7 +11843,7 @@
       </c>
       <c r="I222" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/c22a596095db4994a5f26ba216b6b968/110-0034144b_datasheet_seapath_130-r.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11916,7 +11916,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mru2.pdf']}</t>
         </is>
       </c>
     </row>
@@ -11957,7 +11957,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mrud.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12041,7 +12041,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mru3.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12110,7 +12110,7 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mrue.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12151,7 +12151,7 @@
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mru5.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mruh.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12267,7 +12267,7 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mru5mkii.pdf']}</t>
         </is>
       </c>
     </row>
@@ -12343,7 +12343,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>(nan, nan)</t>
+          <t>{'Data sheet': ['https://www.kongsberg.com/contentassets/77678b37b4c94d51bbfd7d8abdf82c73/datasheet_mrus.pdf']}</t>
         </is>
       </c>
     </row>

</xml_diff>